<commit_message>
Update to week 10 homework
</commit_message>
<xml_diff>
--- a/week-ten/Power usage.xlsx
+++ b/week-ten/Power usage.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://athousandprojects-my.sharepoint.com/personal/graeme_athousandprojects_com/Documents/Study/Making Embedded Systems/making-embedded-projects/week-ten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="8_{E26B1D8D-8632-4105-91C3-BB762D40D477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE52F2CE-E570-4F00-AD5D-876935140E83}"/>
+  <xr:revisionPtr revIDLastSave="184" documentId="8_{E26B1D8D-8632-4105-91C3-BB762D40D477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90B396A1-E123-4629-A6EF-D17B7F054941}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="engineering words" sheetId="1" r:id="rId1"/>
     <sheet name="engineering numbers" sheetId="2" r:id="rId2"/>
     <sheet name="design words" sheetId="3" r:id="rId3"/>
     <sheet name="design numbers" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="Estimated Consuption" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,24 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="83">
   <si>
     <t>1. What are the different states the device can be in?</t>
   </si>
   <si>
-    <t>Wordy can be on (display showing) or sleeping (processor asleep, accelerometer set interrupt/wake it).</t>
-  </si>
-  <si>
     <t>2. How much will your device be in each state?</t>
   </si>
   <si>
-    <t>My goal is for the ring to be on for 5-10s every five minutes. Sometimes it will be on more, as I play with it a lot. More often it will be sleeping, such as left on a table overnight.</t>
-  </si>
-  <si>
     <t>3. How much current is used in each state?</t>
-  </si>
-  <si>
-    <t>Using a DVM in current sensing mode to measure the current in each state.</t>
   </si>
   <si>
     <t>4. How long will the device last given a 40mAh battery?</t>
@@ -272,14 +263,41 @@
   </si>
   <si>
     <t>Duration (h)</t>
+  </si>
+  <si>
+    <t>Operational : Calculating Orentation, time and configuration
+Sleep : wake on Gyro/Acc, RTC or Battery monitor interrupt</t>
+  </si>
+  <si>
+    <t>99% of time will be in sleep mode. Operational time could be limited to &lt;10s or greater when configuring, however, confiuration is not performed offten. There would be a daily download on infotrmaation  +- 10s</t>
+  </si>
+  <si>
+    <t>Using a DVM in current sensing mode to measure the current in each state.
+Using typical figures from datasheets</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Estimating 10 task changes per day @ 10s per task change</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Seconds in day</t>
+  </si>
+  <si>
+    <t>standyBy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="171" formatCode="0.0000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -358,12 +376,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFD9EAD3"/>
         <bgColor rgb="FFD9EAD3"/>
       </patternFill>
@@ -372,6 +384,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD0E0E3"/>
         <bgColor rgb="FFD0E0E3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -384,10 +402,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -404,31 +423,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -746,7 +770,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -761,7 +785,7 @@
     </row>
     <row r="2" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -769,12 +793,12 @@
     </row>
     <row r="4" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -782,26 +806,26 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <f>'engineering numbers'!B26</f>
-        <v>4.9836601307189543</v>
+        <f>'engineering numbers'!C28</f>
+        <v>7.7482313800960334</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3781,179 +3805,261 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="str">
         <f>'engineering words'!A1</f>
         <v>1. What are the different states the device can be in?</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="11"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="str">
         <f>'engineering words'!A4</f>
         <v>2. How much will your device be in each state?</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="B5" s="11"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6">
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="11">
+        <v>86400</v>
+      </c>
+      <c r="D7" s="11"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="5">
-        <f>B7/(SUM(B7:B8))</f>
-        <v>1.6393442622950821E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="B8" s="11"/>
+      <c r="C8" s="6">
+        <v>100</v>
+      </c>
+      <c r="D8" s="27">
+        <f>C8/$C$7</f>
+        <v>1.1574074074074073E-3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="11">
         <v>9</v>
       </c>
-      <c r="B8" s="7">
-        <f>60*5</f>
-        <v>300</v>
-      </c>
-      <c r="C8" s="8">
-        <f>B8/(SUM(B7:B8))</f>
-        <v>0.98360655737704916</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="str">
+      <c r="C9" s="7">
+        <f>B9*(60*60)</f>
+        <v>32400</v>
+      </c>
+      <c r="D9" s="27">
+        <f t="shared" ref="D9:D10" si="0">C9/$C$7</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="29">
+        <f>C7-SUM(C8:C9)</f>
+        <v>53900</v>
+      </c>
+      <c r="D10" s="27">
+        <f t="shared" si="0"/>
+        <v>0.62384259259259256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D11" s="28">
+        <f>SUM(D8:D10)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="str">
         <f>'engineering words'!A7</f>
         <v>3. How much current is used in each state?</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="6">
-        <v>12</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="11"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="6">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="str">
+        <v>5</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="6">
+        <f>'Estimated Consuption'!B21</f>
+        <v>67.417000000000002</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="6">
+        <f>'Estimated Consuption'!C21</f>
+        <v>28.456</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="29">
+        <f>'Estimated Consuption'!D21</f>
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="str">
         <f>'engineering words'!A10</f>
         <v>4. How long will the device last given a 40mAh battery?</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="B18" s="11"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="6">
+        <v>2000</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="25">
+        <f t="shared" ref="C22:C23" si="1">C14*D8</f>
+        <v>7.802893518518518E-2</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="6">
-        <v>40</v>
-      </c>
-      <c r="C18" s="5" t="s">
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="25">
+        <f>C15*D9</f>
+        <v>10.670999999999999</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="11"/>
+      <c r="C24" s="25">
+        <f>C16*D10</f>
+        <v>6.1136574074074071E-3</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="B25" s="11"/>
+      <c r="C25" s="25">
+        <f>SUM(C22:C24)</f>
+        <v>10.755142592592593</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="5"/>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21">
-        <f t="shared" ref="B21:B22" si="0">B13*C7</f>
-        <v>0.19672131147540983</v>
-      </c>
-      <c r="C21" s="5" t="s">
+    </row>
+    <row r="27" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <f>C19/C25</f>
+        <v>185.9575531223048</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>0.13770491803278689</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+    <row r="28" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C28" s="9">
+        <f>C27/24</f>
+        <v>7.7482313800960334</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="B23">
-        <f>SUM(B21:B22)</f>
-        <v>0.33442622950819673</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B25">
-        <f>B18/B23</f>
-        <v>119.6078431372549</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B26" s="10">
-        <f>B25/24</f>
-        <v>4.9836601307189543</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -3979,12 +4085,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3992,12 +4098,12 @@
     </row>
     <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4005,22 +4111,22 @@
     </row>
     <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>29</v>
+      <c r="A11" s="10" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7002,7 +7108,9 @@
   </sheetPr>
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7010,17 +7118,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
-        <v>22</v>
+      <c r="A1" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <v>5</v>
       </c>
     </row>
@@ -7029,45 +7137,45 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="14">
+        <v>2000</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="14">
+        <v>3.7</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="15">
-        <v>40</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="15">
-        <v>3.7</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="15"/>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
-        <v>24</v>
+      <c r="A10" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B11" s="6">
         <v>48</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7078,48 +7186,48 @@
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="17">
+      <c r="A15" s="16">
         <f>A7/B11</f>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>13</v>
+        <v>41.666666666666664</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="19" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B20" s="5">
         <v>0.25</v>
@@ -7128,15 +7236,15 @@
         <v>0.09</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>45</v>
+        <v>10</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B21" s="5">
         <v>0.3</v>
@@ -7145,15 +7253,15 @@
         <v>1E-3</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>47</v>
+        <v>10</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B22" s="5">
         <v>0.6</v>
@@ -7162,15 +7270,15 @@
         <v>0.08</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>49</v>
+        <v>10</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B23" s="5">
         <v>12</v>
@@ -7179,15 +7287,15 @@
         <v>0</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B24" s="5">
         <v>0.16500000000000001</v>
@@ -7196,15 +7304,15 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>53</v>
+        <v>10</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B26">
         <f t="shared" ref="B26:C26" si="0">SUM(B20:B24)</f>
@@ -7215,28 +7323,28 @@
         <v>0.17699999999999999</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" s="17">
+      <c r="A27" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="16">
         <f>A7/B26</f>
-        <v>3.0041306796845664</v>
-      </c>
-      <c r="C27" s="17">
+        <v>150.20653398422832</v>
+      </c>
+      <c r="C27" s="16">
         <f>A7/C26</f>
-        <v>225.98870056497177</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>36</v>
+        <v>11299.435028248588</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -7244,14 +7352,14 @@
         <v>5</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D30">
         <f>(B30/100)*B26 + (1-(B30/10))*C26</f>
         <v>0.75425000000000009</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -7259,24 +7367,24 @@
         <v>10</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D31">
         <f>(B31/100)*B26 + (1-(B31/10))*C26</f>
         <v>1.3315000000000001</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A34" s="22" t="s">
-        <v>29</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="21" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -7293,63 +7401,62 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59ADF3FF-F8EE-4B14-94E1-C7C627007A7A}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
-        <v>66</v>
-      </c>
-    </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="24" t="s">
-        <v>67</v>
+      <c r="A5" s="23" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>69</v>
+        <v>61</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
-        <v>61</v>
+      <c r="A11" s="22" t="s">
+        <v>58</v>
       </c>
       <c r="B11">
         <v>31.1</v>
@@ -7357,30 +7464,42 @@
       <c r="C11">
         <v>12.2</v>
       </c>
-      <c r="D11">
-        <v>0.112</v>
-      </c>
-      <c r="E11" s="24">
+      <c r="D11" s="23">
         <f>2.8/1000</f>
         <v>2.8E-3</v>
       </c>
+      <c r="E11">
+        <v>0.112</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="23" t="s">
-        <v>70</v>
+      <c r="B13" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="26">
+        <v>0.25</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
-        <v>75</v>
+      <c r="A14" s="22" t="s">
+        <v>72</v>
       </c>
       <c r="B14">
         <v>36.299999999999997</v>
       </c>
+      <c r="C14">
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <v>1E-3</v>
+      </c>
+      <c r="E14">
+        <v>1.0009999999999999</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
-        <v>71</v>
+      <c r="A16" s="22" t="s">
+        <v>68</v>
       </c>
       <c r="B16">
         <f>3/1000</f>
@@ -7390,18 +7509,32 @@
         <f>1/1000</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="23" t="s">
-        <v>72</v>
+      <c r="D16">
+        <f t="shared" ref="D16:E16" si="0">1/1000</f>
+        <v>1E-3</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="22" t="s">
+        <v>69</v>
       </c>
       <c r="B19">
         <f>14/1000</f>
@@ -7411,28 +7544,93 @@
         <f>5/1000</f>
         <v>5.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="25">
+      <c r="D19">
+        <f t="shared" ref="D19:E19" si="1">5/1000</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="24">
         <f>SUM(B11:B20)</f>
         <v>67.417000000000002</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" s="24">
+      <c r="C21" s="24">
+        <f>SUM(C11:C20)</f>
+        <v>28.456</v>
+      </c>
+      <c r="D21" s="24">
+        <f t="shared" ref="D21" si="2">SUM(D11:D20)</f>
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="E21" s="24">
+        <f>SUM(E11:E20)</f>
+        <v>1.1189999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="23">
         <v>2000</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="24" t="s">
-        <v>77</v>
+      <c r="C23" s="23">
+        <v>2001</v>
+      </c>
+      <c r="D23" s="23">
+        <v>2003</v>
+      </c>
+      <c r="E23" s="23">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="23" t="s">
+        <v>74</v>
       </c>
       <c r="B24">
         <f>B23/B21</f>
         <v>29.666107954966847</v>
+      </c>
+      <c r="C24">
+        <f>C23/C21</f>
+        <v>70.319089120044978</v>
+      </c>
+      <c r="D24">
+        <f t="shared" ref="D24" si="3">D23/D21</f>
+        <v>204387.75510204083</v>
+      </c>
+      <c r="E24">
+        <f>E23/E21</f>
+        <v>1789.0974084003578</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25">
+        <f>B24/24</f>
+        <v>1.2360878314569519</v>
+      </c>
+      <c r="C25">
+        <f>C24/24</f>
+        <v>2.9299620466685408</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ref="D25" si="4">D24/24</f>
+        <v>8516.1564625850351</v>
+      </c>
+      <c r="E25">
+        <f>E24/24</f>
+        <v>74.545725350014905</v>
       </c>
     </row>
   </sheetData>

</xml_diff>